<commit_message>
Completed new version of sankey diagram (figure 2)
</commit_message>
<xml_diff>
--- a/glass_paper.xlsx
+++ b/glass_paper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jose\Desktop\python\glass-paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB1314C1-547A-468E-B55A-6800CDDE953D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38272F5B-6C8D-446D-8076-31F901D3B157}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{1AC0E601-1297-4C8D-8E5F-6A8C787FDED8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="83">
   <si>
     <t>Global production of glass</t>
   </si>
@@ -131,12 +131,6 @@
     <t>Estimated</t>
   </si>
   <si>
-    <t>Target</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
     <t>Value</t>
   </si>
   <si>
@@ -146,12 +140,6 @@
     <t>Soda Ash</t>
   </si>
   <si>
-    <t>FG Batch</t>
-  </si>
-  <si>
-    <t>Batch preparation</t>
-  </si>
-  <si>
     <t>Limestone (CaCO3)</t>
   </si>
   <si>
@@ -167,12 +155,6 @@
     <t>Batch-to-Melt Yield</t>
   </si>
   <si>
-    <t>CG Cullet</t>
-  </si>
-  <si>
-    <t>CG Batch</t>
-  </si>
-  <si>
     <t>Cont Fabrication Yield Loss</t>
   </si>
   <si>
@@ -185,45 +167,21 @@
     <t>End-use CG Food</t>
   </si>
   <si>
-    <t>Int CG</t>
-  </si>
-  <si>
-    <t>Melting</t>
-  </si>
-  <si>
     <t>End-use CG Other</t>
   </si>
   <si>
-    <t>CG Process Emissions</t>
-  </si>
-  <si>
     <t>End-use FG Buildings</t>
   </si>
   <si>
-    <t>Int FG</t>
-  </si>
-  <si>
     <t>End-use FG Automotive</t>
   </si>
   <si>
-    <t>FG Process Emissions</t>
-  </si>
-  <si>
     <t>End-use FG Other FG</t>
   </si>
   <si>
-    <t>Final CG</t>
-  </si>
-  <si>
-    <t>Checking</t>
-  </si>
-  <si>
     <t>Global Cont Recycling Rate</t>
   </si>
   <si>
-    <t>Final FG</t>
-  </si>
-  <si>
     <t>Global Cont Landfill Rate</t>
   </si>
   <si>
@@ -233,9 +191,6 @@
     <t>Beverages</t>
   </si>
   <si>
-    <t>End-Use</t>
-  </si>
-  <si>
     <t>Container</t>
   </si>
   <si>
@@ -257,12 +212,6 @@
     <t>Other FG</t>
   </si>
   <si>
-    <t>End-of-Life</t>
-  </si>
-  <si>
-    <t>Landfill</t>
-  </si>
-  <si>
     <t>Table 15.6: https://www.sciencedirect.com/science/article/pii/B9780128150603000153</t>
   </si>
   <si>
@@ -285,6 +234,57 @@
   </si>
   <si>
     <t>Poland container glass production [Mt]</t>
+  </si>
+  <si>
+    <t>loss1</t>
+  </si>
+  <si>
+    <t>loss2</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>target</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>RM</t>
+  </si>
+  <si>
+    <t>FGM</t>
+  </si>
+  <si>
+    <t>CGM</t>
+  </si>
+  <si>
+    <t>Liquid glass</t>
+  </si>
+  <si>
+    <t>Emission</t>
+  </si>
+  <si>
+    <t>CGF</t>
+  </si>
+  <si>
+    <t>FGF</t>
+  </si>
+  <si>
+    <t>CGU</t>
+  </si>
+  <si>
+    <t>Forming scrap</t>
+  </si>
+  <si>
+    <t>FGU</t>
+  </si>
+  <si>
+    <t>EoL</t>
   </si>
 </sst>
 </file>
@@ -741,7 +741,7 @@
   <dimension ref="B2:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -757,7 +757,7 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
@@ -765,7 +765,7 @@
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="C3">
         <v>2014</v>
@@ -774,12 +774,12 @@
         <v>77</v>
       </c>
       <c r="E3" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="C4">
         <v>2007</v>
@@ -788,12 +788,12 @@
         <v>72</v>
       </c>
       <c r="E4" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="C5">
         <v>2007</v>
@@ -808,7 +808,7 @@
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="C6">
         <v>2014</v>
@@ -823,7 +823,7 @@
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="C7">
         <v>2014</v>
@@ -838,7 +838,7 @@
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="C8">
         <v>2007</v>
@@ -852,7 +852,7 @@
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="C9">
         <v>2014</v>
@@ -866,7 +866,7 @@
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="C10">
         <v>2007</v>
@@ -880,7 +880,7 @@
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="C11">
         <v>2014</v>
@@ -916,7 +916,7 @@
   <dimension ref="B2:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -933,7 +933,7 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
@@ -1179,31 +1179,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11B3549B-C2AB-4D75-AB88-A04A3C1A4639}">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
     <col min="7" max="7" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>68</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="C1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" t="s">
         <v>32</v>
-      </c>
-      <c r="D1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G1" t="s">
-        <v>34</v>
       </c>
       <c r="H1" s="5">
         <v>0.22409999999999999</v>
@@ -1211,20 +1212,20 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="2">
-        <f>((D14+D12))*H1</f>
+        <v>33</v>
+      </c>
+      <c r="D2" s="4">
+        <f>(('Flat glass'!D19+D12))*H1</f>
         <v>18.776050481185038</v>
       </c>
       <c r="G2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H2" s="5">
         <v>0.14069999999999999</v>
@@ -1232,20 +1233,20 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="B3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="4">
+        <f>(('Flat glass'!D19+D12))*H3</f>
+        <v>53.219755759253616</v>
+      </c>
+      <c r="G3" t="s">
         <v>36</v>
-      </c>
-      <c r="C3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="2">
-        <f>((D14+D12))*H3</f>
-        <v>53.219755759253616</v>
-      </c>
-      <c r="G3" t="s">
-        <v>40</v>
       </c>
       <c r="H3" s="5">
         <v>0.63519999999999999</v>
@@ -1253,41 +1254,29 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="C4" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="2">
-        <f>((D14+D12))*H2</f>
+      <c r="D4" s="4">
+        <f>(('Flat glass'!D19+D12))*H2</f>
         <v>11.788444010275478</v>
       </c>
       <c r="G4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="H4" s="5">
         <v>0.84530000000000005</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" s="2">
-        <f>SUM(D23:D25)</f>
-        <v>27.597623836290182</v>
-      </c>
+      <c r="D5" s="4"/>
       <c r="G5" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="H5" s="5">
         <v>0.1</v>
@@ -1295,20 +1284,20 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>72</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="2">
-        <f>((D13+D10)-(D5))*H1</f>
+        <v>33</v>
+      </c>
+      <c r="D6" s="4">
+        <f>(('Container glass'!D13+D10)-(SUM(D23:D25)))*H1</f>
         <v>13.58776385767761</v>
       </c>
       <c r="G6" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="H6" s="5">
         <v>0.15</v>
@@ -1316,20 +1305,20 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="2">
-        <f>((D13+D10)-(D5))*H3</f>
+        <v>35</v>
+      </c>
+      <c r="D7" s="4">
+        <f>(('Container glass'!D13+D10)-(SUM(D23:D25)))*H3</f>
         <v>38.513822411409272</v>
       </c>
       <c r="G7" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="H7" s="5">
         <v>0.75</v>
@@ -1337,20 +1326,20 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
       <c r="C8" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="2">
-        <f>((D13+D10)-(D5))*H2</f>
+      <c r="D8" s="4">
+        <f>(('Container glass'!D13+D10)-(SUM(D23:D25)))*H2</f>
         <v>8.5310056884214163</v>
       </c>
       <c r="G8" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="H8" s="5">
         <v>0.2</v>
@@ -1358,20 +1347,20 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9" s="2">
-        <f>D13/(1-H5)</f>
+        <v>75</v>
+      </c>
+      <c r="D9" s="4">
+        <f>SUM(D17:D19)/(1-H5)</f>
         <v>87.61150424219106</v>
       </c>
       <c r="G9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="H9" s="5">
         <v>0.05</v>
@@ -1379,20 +1368,20 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="4">
+        <f>(('Container glass'!D13-SUM(D23:D25))/H4)*(1-H4)</f>
+        <v>9.3798619758265307</v>
+      </c>
+      <c r="G10" t="s">
         <v>44</v>
-      </c>
-      <c r="B10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" s="2">
-        <f>((D13-D5)/H4)*(1-H4)</f>
-        <v>9.3798619758265307</v>
-      </c>
-      <c r="G10" t="s">
-        <v>53</v>
       </c>
       <c r="H10" s="5">
         <v>0.83</v>
@@ -1400,20 +1389,20 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="B11" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="2">
-        <f>D14/(1-H6)</f>
+        <v>75</v>
+      </c>
+      <c r="D11" s="4">
+        <f>'Flat glass'!D19/(1-H6)</f>
         <v>83.320972631680775</v>
       </c>
       <c r="G11" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="H11" s="5">
         <v>0.06</v>
@@ -1421,62 +1410,38 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="B12" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" s="2">
-        <f>(D14/H4)*(1-H4)</f>
+        <v>76</v>
+      </c>
+      <c r="D12" s="4">
+        <f>('Flat glass'!D19/H4)*(1-H4)</f>
         <v>12.961423513785473</v>
       </c>
       <c r="G12" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="H12" s="5">
         <v>0.11</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>49</v>
-      </c>
-      <c r="B13" t="s">
-        <v>58</v>
-      </c>
-      <c r="C13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D13" s="2">
-        <f>'Container glass'!D13</f>
-        <v>78.85035381797195</v>
-      </c>
+      <c r="D13" s="4"/>
       <c r="G13" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="H13" s="6">
         <v>0.35</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>54</v>
-      </c>
-      <c r="B14" t="s">
-        <v>61</v>
-      </c>
-      <c r="C14" t="s">
-        <v>59</v>
-      </c>
-      <c r="D14" s="2">
-        <f>'Flat glass'!D19</f>
-        <v>70.822826736928661</v>
-      </c>
+      <c r="D14" s="4"/>
       <c r="G14" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="H14" s="6">
         <v>0.65</v>
@@ -1484,53 +1449,53 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
       <c r="C15" t="s">
-        <v>59</v>
-      </c>
-      <c r="D15" s="2">
-        <f>(D13/(1-H5))-D13</f>
+        <v>80</v>
+      </c>
+      <c r="D15" s="4">
+        <f>(SUM(D17:D19)/(1-H5))-SUM(D17:D19)</f>
         <v>8.7611504242191103</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="C16" t="s">
-        <v>59</v>
-      </c>
-      <c r="D16" s="2">
-        <f>(D14/(1-H6))-D14</f>
+        <v>80</v>
+      </c>
+      <c r="D16" s="4">
+        <f>('Flat glass'!D19/(1-H6))-'Flat glass'!D19</f>
         <v>12.498145894752113</v>
       </c>
       <c r="G16" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="B17" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="C17" t="s">
-        <v>65</v>
-      </c>
-      <c r="D17" s="2">
-        <f>D13*H7</f>
+        <v>50</v>
+      </c>
+      <c r="D17" s="4">
+        <f>'Container glass'!D13*H7</f>
         <v>59.137765363478962</v>
       </c>
       <c r="G17" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="H17" s="5">
         <v>0.37490000000000001</v>
@@ -1538,20 +1503,20 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="B18" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C18" t="s">
-        <v>65</v>
-      </c>
-      <c r="D18" s="2">
-        <f>D13*H8</f>
+        <v>52</v>
+      </c>
+      <c r="D18" s="4">
+        <f>'Container glass'!D13*H8</f>
         <v>15.77007076359439</v>
       </c>
       <c r="G18" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="H18" s="5">
         <v>0.1298</v>
@@ -1559,188 +1524,188 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="B19" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="C19" t="s">
-        <v>65</v>
-      </c>
-      <c r="D19" s="2">
-        <f>D13*H9</f>
+        <v>54</v>
+      </c>
+      <c r="D19" s="4">
+        <f>'Container glass'!D13*H9</f>
         <v>3.9425176908985975</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="B20" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="C20" t="s">
-        <v>65</v>
-      </c>
-      <c r="D20" s="2">
-        <f>D14*H10</f>
+        <v>55</v>
+      </c>
+      <c r="D20" s="4">
+        <f>'Flat glass'!D19*H10</f>
         <v>58.782946191650787</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="B21" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="C21" t="s">
-        <v>65</v>
-      </c>
-      <c r="D21" s="2">
-        <f>D14*H11</f>
+        <v>56</v>
+      </c>
+      <c r="D21" s="4">
+        <f>'Flat glass'!D19*H11</f>
         <v>4.2493696042157199</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="B22" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="C22" t="s">
-        <v>65</v>
-      </c>
-      <c r="D22" s="2">
-        <f>D14*H12</f>
+        <v>57</v>
+      </c>
+      <c r="D22" s="4">
+        <f>'Flat glass'!D19*H12</f>
         <v>7.7905109410621529</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="C23" t="s">
-        <v>73</v>
-      </c>
-      <c r="D23" s="2">
+        <v>50</v>
+      </c>
+      <c r="D23" s="4">
         <f>D17*H13</f>
         <v>20.698217877217637</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="C24" t="s">
-        <v>73</v>
-      </c>
-      <c r="D24" s="2">
+        <v>52</v>
+      </c>
+      <c r="D24" s="4">
         <f>D18*H13</f>
         <v>5.5195247672580363</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B25" t="s">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="C25" t="s">
-        <v>73</v>
-      </c>
-      <c r="D25" s="2">
+        <v>54</v>
+      </c>
+      <c r="D25" s="4">
         <f>D19*H13</f>
         <v>1.3798811918145091</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="B26" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C26" t="s">
-        <v>73</v>
-      </c>
-      <c r="D26" s="2">
+        <v>50</v>
+      </c>
+      <c r="D26" s="4">
         <f>D17*H14</f>
         <v>38.439547486261326</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="B27" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C27" t="s">
-        <v>73</v>
-      </c>
-      <c r="D27" s="2">
+        <v>52</v>
+      </c>
+      <c r="D27" s="4">
         <f>D18*H14</f>
         <v>10.250545996336355</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B28" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C28" t="s">
-        <v>73</v>
-      </c>
-      <c r="D28" s="2">
+        <v>54</v>
+      </c>
+      <c r="D28" s="4">
         <f>D19*H14</f>
         <v>2.5626364990840886</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="B29" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C29" t="s">
-        <v>73</v>
-      </c>
-      <c r="D29">
+        <v>55</v>
+      </c>
+      <c r="D29" s="4">
         <f>4.3+2.7+12.5+0.4+0.4+0.1</f>
         <v>20.399999999999999</v>
       </c>
       <c r="E29" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B30" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C30" t="s">
-        <v>73</v>
-      </c>
-      <c r="D30" s="2">
+        <v>56</v>
+      </c>
+      <c r="D30" s="4">
         <f>(0.15+0.25+0.08+0.1)*100/(15+16+16+28)</f>
         <v>0.77333333333333343</v>
       </c>
       <c r="E30" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>